<commit_message>
first try at a case, HVPS voltage calc
</commit_message>
<xml_diff>
--- a/resources/1363_Radj.xlsx
+++ b/resources/1363_Radj.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +385,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>169.5</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -397,7 +397,7 @@
       </c>
       <c r="B3">
         <f>(-1.24/(0.124-((B2-1.24)/1208))) - 30.1</f>
-        <v>51.0089452025125</v>
+        <v>77.139404352806537</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>

</xml_diff>